<commit_message>
archivo CSS completo y corregido,  estética uniforme en toda la aplicación.
</commit_message>
<xml_diff>
--- a/spreadsheets/datos.xlsx
+++ b/spreadsheets/datos.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -880,17 +880,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>anillo oro 18 k piedra rubi oval sello</t>
+          <t>sello letra F M ORO 18 K</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>400</t>
         </is>
       </c>
       <c r="E14" s="1" t="inlineStr">
@@ -912,17 +912,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>sello letra F M ORO 18 K</t>
+          <t>Pulsera oro 18 k 4 monedas</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>65</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>6000</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr">
@@ -949,22 +949,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>53</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>6000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F16" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -976,22 +971,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Pulsera oro 18 k 4 monedas</t>
+          <t>Pulsera oro 18 k medalla cierre de seguridad</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>2500</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1003,17 +1003,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Pulsera oro 18 k medalla cierre de seguridad</t>
+          <t>Pulsera oro 18 k 4 monedas</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>49</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr">
@@ -1035,17 +1035,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Pulsera oro 18 k 4 monedas</t>
+          <t>correa reloj oro 18 k</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>38</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr">
@@ -1067,17 +1067,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>correa reloj oro 18 k</t>
+          <t>reloj cyma de oro antiguo</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>33</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr">
@@ -1088,6 +1088,11 @@
       <c r="F20" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 2</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 3</t>
         </is>
       </c>
     </row>
@@ -1099,17 +1104,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>reloj cyma de oro antiguo</t>
+          <t>pulsera rigida oro 18 k labrada</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>58</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>6000</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr">
@@ -1141,7 +1146,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>54</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1178,12 +1183,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>44</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>6000</t>
+          <t>5500</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr">
@@ -1210,32 +1215,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>pulsera rigida oro 18 k labrada</t>
+          <t>pendientes oro 18 k hoja</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>5500</t>
+          <t>150</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F24" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
-        </is>
-      </c>
-      <c r="G24" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 3</t>
         </is>
       </c>
     </row>
@@ -1247,22 +1242,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>pendientes oro 18 k hoja</t>
+          <t>juego pendientes y anillo oro y granate rojo</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>500</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1274,27 +1274,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>juego pendientes y anillo oro y granate rojo</t>
+          <t>cadenas y pieza dental oro</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>16</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F26" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1306,22 +1301,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>cadenas y pieza dental oro</t>
+          <t>3 medallas y cruz carabaca con cadena</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1333,27 +1333,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3 medallas y cruz carabaca con cadena</t>
+          <t>collar oro 18 kilates y coral</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1310</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F28" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1365,17 +1360,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>collar oro 18 kilates y coral</t>
+          <t>pulsera oro 18 k y coral</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1310</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr">
@@ -1392,7 +1387,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>pulsera oro 18 k y coral</t>
+          <t>juego de pendiente y anillo oro y coral</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1402,12 +1397,22 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1200</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
+      </c>
+      <c r="G30" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 3</t>
         </is>
       </c>
     </row>
@@ -1419,17 +1424,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>juego de pendiente y anillo oro y coral</t>
+          <t xml:space="preserve">pulsera oro dibujo trenzado </t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1200</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr">
@@ -1440,11 +1445,6 @@
       <c r="F31" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 2</t>
-        </is>
-      </c>
-      <c r="G31" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 3</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">pulsera oro dibujo trenzado </t>
+          <t>3 anillos unidos piedra oro 18 k</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>300</t>
         </is>
       </c>
       <c r="E32" s="1" t="inlineStr">
@@ -1488,12 +1488,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3 anillos unidos piedra oro 18 k</t>
+          <t>anillo de oro piedra cuarzo ahumado rectangular</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1520,12 +1520,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>anillo de oro piedra cuarzo ahumado rectangular</t>
+          <t>anillo sw oro 18 k. y muchas circonitas</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1552,27 +1552,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>anillo sw oro 18 k. y muchas circonitas</t>
+          <t>2 alianzas de oro 18 k</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>150</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F35" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1584,7 +1579,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2 alianzas de oro 18 k</t>
+          <t>2 pendientes oro circonitas y perlita</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1600,6 +1595,11 @@
       <c r="E36" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1611,27 +1611,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2 pendientes oro circonitas y perlita</t>
+          <t>reloj cyma de oro</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>29</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E37" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F37" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1643,22 +1638,27 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>reloj cyma de oro</t>
+          <t>juego de pendientes y anillo oro circonitas y rubi</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1670,17 +1670,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>juego de pendientes y anillo oro circonitas y rubi</t>
+          <t xml:space="preserve">guardapelo, cruz cadena globo fetiche </t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr">
@@ -1702,17 +1702,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">guardapelo, cruz cadena globo fetiche </t>
+          <t>sortija oro blanco y amarillo con perla y brillantes</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="E40" s="1" t="inlineStr">
@@ -1734,27 +1734,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>sortija oro blanco y amarillo con perla y brillantes</t>
+          <t>collar de perlas en disminucion con cierre de oro</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>300</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F41" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1766,22 +1761,27 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>collar de perlas en disminucion con cierre de oro</t>
+          <t>reloj de oro cronwell</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>34</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>4000</t>
         </is>
       </c>
       <c r="E42" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1793,17 +1793,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>reloj de oro cronwell</t>
+          <t>reloj de oro cyma (mama)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>47</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4000</t>
+          <t>3000</t>
         </is>
       </c>
       <c r="E43" s="1" t="inlineStr">
@@ -1825,27 +1825,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>reloj de oro cyma (mama)</t>
+          <t>reloj omega sra. Constelacion</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>8000</t>
         </is>
       </c>
       <c r="E44" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F44" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1857,22 +1852,32 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>reloj omega sra. Constelacion</t>
+          <t>sortija  oro amarillo y blanco con un gran diamante</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>8000</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="E45" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
+      </c>
+      <c r="G45" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 3</t>
         </is>
       </c>
     </row>
@@ -1884,32 +1889,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>sortija  oro amarillo y blanco con un gran diamante</t>
+          <t>placa eugenio de frutos oro</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>240</t>
         </is>
       </c>
       <c r="E46" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F46" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
-        </is>
-      </c>
-      <c r="G46" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 3</t>
         </is>
       </c>
     </row>
@@ -1921,22 +1916,27 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>placa eugenio de frutos oro</t>
+          <t>anillo de oro blanco y diamantes</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="E47" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>anillo de oro blanco y diamantes</t>
+          <t>pendientes oro blanco y diamante</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1964,11 +1964,6 @@
       <c r="E48" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F48" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -1980,17 +1975,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>pendientes oro blanco y diamante</t>
+          <t>pendientes oro blanco y brillantes largos</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>800</t>
         </is>
       </c>
       <c r="E49" s="1" t="inlineStr">
@@ -2007,17 +2002,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>pendientes oro blanco y brillantes largos</t>
+          <t xml:space="preserve">pulsera oro blanco y circonitas </t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="E50" s="1" t="inlineStr">
@@ -2034,17 +2029,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve">pulsera oro blanco y circonitas </t>
+          <t xml:space="preserve">3 pulseras oro </t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>38</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>3000</t>
         </is>
       </c>
       <c r="E51" s="1" t="inlineStr">
@@ -2061,22 +2056,27 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 pulseras oro </t>
+          <t>pulsera antigua oro amarillo y blanco con brillantes</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>2500</t>
         </is>
       </c>
       <c r="E52" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -2088,12 +2088,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>pulsera antigua oro amarillo y blanco con brillantes</t>
+          <t xml:space="preserve">cadena y colgante oro blanco con diamantesy perla </t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2120,27 +2120,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve">cadena y colgante oro blanco con diamantesy perla </t>
+          <t>cadena y cruz oro (papa)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>16</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="E54" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F54" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -2152,17 +2147,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>cadena y cruz oro (papa)</t>
+          <t xml:space="preserve">cadena oro y colgante tous </t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>300</t>
         </is>
       </c>
       <c r="E55" s="1" t="inlineStr">
@@ -2179,12 +2174,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve">cadena oro y colgante tous </t>
+          <t>cadena y cruz oeo blanco (boda)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2206,17 +2201,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>cadena y cruz oeo blanco (boda)</t>
+          <t>medalla virgen y cruz con cadena oro 18 k (Mari)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>1200</t>
         </is>
       </c>
       <c r="E57" s="1" t="inlineStr">
@@ -2233,17 +2228,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>medalla virgen y cruz con cadena oro 18 k (Mari)</t>
+          <t>pulsera oro 18 k y perlas (Mari)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1200</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E58" s="1" t="inlineStr">
@@ -2260,17 +2255,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>pulsera oro 18 k y perlas (Mari)</t>
+          <t>pulsera aro oro 18 k (regalo Tere)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>500</t>
         </is>
       </c>
       <c r="E59" s="1" t="inlineStr">
@@ -2287,17 +2282,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>pulsera aro oro 18 k (regalo Tere)</t>
+          <t xml:space="preserve">Gargantilla trenzada oro 18 k </t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E60" s="1" t="inlineStr">
@@ -2314,17 +2309,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gargantilla trenzada oro 18 k </t>
+          <t>gargantilla perlas de rio con broche de oro</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>200</t>
         </is>
       </c>
       <c r="E61" s="1" t="inlineStr">
@@ -2341,17 +2336,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>gargantilla perlas de rio con broche de oro</t>
+          <t>cadena y cruz pequeña oro 18 k</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>160</t>
         </is>
       </c>
       <c r="E62" s="1" t="inlineStr">
@@ -2368,22 +2363,27 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>cadena y cruz pequeña oro 18 k</t>
+          <t>anillo de oro blanco y amarillo 3 brillantes</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>1200</t>
         </is>
       </c>
       <c r="E63" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F63" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>anillo de oro blanco y amarillo 3 brillantes</t>
+          <t>sortija oro 18k circonitas y rubis</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2405,17 +2405,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1200</t>
+          <t>240</t>
         </is>
       </c>
       <c r="E64" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F64" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -2427,22 +2422,27 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>sortija oro 18k circonitas y rubis</t>
+          <t>sortija oro 18k aro grueso</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>880</t>
         </is>
       </c>
       <c r="E65" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F65" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -2454,17 +2454,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>sortija oro 18k aro grueso</t>
+          <t>sortija oro 18k  y circonitas (joyeria Juanjo)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>880</t>
+          <t>400</t>
         </is>
       </c>
       <c r="E66" s="1" t="inlineStr">
@@ -2486,17 +2486,17 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>sortija oro 18k  y circonitas (joyeria Juanjo)</t>
+          <t>solitario oro 18k  con un brillante (joyeria Juanjo)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>600</t>
         </is>
       </c>
       <c r="E67" s="1" t="inlineStr">
@@ -2518,17 +2518,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>solitario oro 18k  con un brillante (joyeria Juanjo)</t>
+          <t>sello oro 18k EG (papa)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>1600</t>
         </is>
       </c>
       <c r="E68" s="1" t="inlineStr">
@@ -2550,17 +2550,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>sello oro 18k EG (papa)</t>
+          <t>sortija oro blabco y amarillo con circonitas</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1600</t>
+          <t>400</t>
         </is>
       </c>
       <c r="E69" s="1" t="inlineStr">
@@ -2582,27 +2582,22 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>sortija oro blabco y amarillo con circonitas</t>
+          <t>anillo oro 18k con dos circonitas (joyeria Juanjo)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>240</t>
         </is>
       </c>
       <c r="E70" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F70" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -2614,23 +2609,14 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>anillo oro 18k con dos circonitas (joyeria Juanjo)</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
-      </c>
-      <c r="E71" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 1</t>
-        </is>
+          <t>anillo oro blanco y amarillo con un brillante (17/03/02)</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>3</v>
+      </c>
+      <c r="D71" t="n">
+        <v>400</v>
       </c>
     </row>
     <row r="72">
@@ -2641,14 +2627,28 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>anillo oro blanco y amarillo con un brillante (17/03/02)</t>
-        </is>
-      </c>
-      <c r="C72" t="n">
-        <v>3</v>
-      </c>
-      <c r="D72" t="n">
-        <v>400</v>
+          <t xml:space="preserve">alianza Mama </t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="E72" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 1</t>
+        </is>
+      </c>
+      <c r="F72" s="1" t="inlineStr">
+        <is>
+          <t>Ver Imagen 2</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -2659,27 +2659,22 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t xml:space="preserve">alianza Mama </t>
+          <t>sortija regalo a Eugenio oro b y amarillo 2 brillantes</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>700</t>
         </is>
       </c>
       <c r="E73" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
-        </is>
-      </c>
-      <c r="F73" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 2</t>
         </is>
       </c>
     </row>
@@ -2691,17 +2686,17 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>sortija regalo a Eugenio oro b y amarillo 2 brillantes</t>
+          <t>broche de oro y rubis</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>480</t>
         </is>
       </c>
       <c r="E74" s="1" t="inlineStr">
@@ -2718,17 +2713,17 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>broche de oro y rubis</t>
+          <t>juego de pendientes agua marina oro blanco</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>480</t>
+          <t>1200</t>
         </is>
       </c>
       <c r="E75" s="1" t="inlineStr">
@@ -2740,7 +2735,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>75</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2767,7 +2762,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>76</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2794,7 +2789,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>77</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2821,7 +2816,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>79</t>
+          <t>78</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2848,7 +2843,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>79</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2875,7 +2870,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>80</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2902,7 +2897,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>81</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2929,7 +2924,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>82</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2956,7 +2951,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>83</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2975,33 +2970,6 @@
         </is>
       </c>
       <c r="E84" s="1" t="inlineStr">
-        <is>
-          <t>Ver Imagen 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>juego de sortija y colgante aguamarina oro blanco</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="E85" s="1" t="inlineStr">
         <is>
           <t>Ver Imagen 1</t>
         </is>
@@ -3042,37 +3010,37 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E15" r:id="rId31"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F15" r:id="rId32"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E16" r:id="rId33"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F16" r:id="rId34"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E17" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E17" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F17" r:id="rId35"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E18" r:id="rId36"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F18" r:id="rId37"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E19" r:id="rId38"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F19" r:id="rId39"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E20" r:id="rId40"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F20" r:id="rId41"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E21" r:id="rId42"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F21" r:id="rId43"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G21" r:id="rId44"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E22" r:id="rId45"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId46"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G22" r:id="rId47"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E23" r:id="rId48"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F23" r:id="rId49"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G23" r:id="rId50"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E24" r:id="rId51"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F24" r:id="rId52"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G24" r:id="rId53"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E25" r:id="rId54"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G20" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E21" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F21" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G21" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E22" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId47"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G22" r:id="rId48"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E23" r:id="rId49"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F23" r:id="rId50"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G23" r:id="rId51"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E24" r:id="rId52"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E25" r:id="rId53"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F25" r:id="rId54"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E26" r:id="rId55"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F26" r:id="rId56"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E27" r:id="rId57"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E27" r:id="rId56"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F27" r:id="rId57"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E28" r:id="rId58"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F28" r:id="rId59"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E29" r:id="rId60"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E30" r:id="rId61"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E31" r:id="rId62"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F31" r:id="rId63"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G31" r:id="rId64"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E29" r:id="rId59"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E30" r:id="rId60"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F30" r:id="rId61"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G30" r:id="rId62"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E31" r:id="rId63"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F31" r:id="rId64"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E32" r:id="rId65"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F32" r:id="rId66"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E33" r:id="rId67"/>
@@ -3080,49 +3048,49 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E34" r:id="rId69"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F34" r:id="rId70"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E35" r:id="rId71"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F35" r:id="rId72"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E36" r:id="rId73"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E36" r:id="rId72"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F36" r:id="rId73"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E37" r:id="rId74"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F37" r:id="rId75"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E38" r:id="rId76"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E38" r:id="rId75"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F38" r:id="rId76"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E39" r:id="rId77"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F39" r:id="rId78"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E40" r:id="rId79"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F40" r:id="rId80"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E41" r:id="rId81"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F41" r:id="rId82"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E42" r:id="rId83"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E42" r:id="rId82"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F42" r:id="rId83"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E43" r:id="rId84"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F43" r:id="rId85"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E44" r:id="rId86"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F44" r:id="rId87"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E45" r:id="rId88"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E46" r:id="rId89"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F46" r:id="rId90"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G46" r:id="rId91"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E47" r:id="rId92"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E45" r:id="rId87"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F45" r:id="rId88"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G45" r:id="rId89"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E46" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E47" r:id="rId91"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F47" r:id="rId92"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E48" r:id="rId93"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F48" r:id="rId94"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E49" r:id="rId95"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E50" r:id="rId96"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E51" r:id="rId97"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E52" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E49" r:id="rId94"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E50" r:id="rId95"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E51" r:id="rId96"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E52" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F52" r:id="rId98"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E53" r:id="rId99"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F53" r:id="rId100"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E54" r:id="rId101"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F54" r:id="rId102"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E55" r:id="rId103"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E56" r:id="rId104"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E57" r:id="rId105"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E58" r:id="rId106"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E59" r:id="rId107"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E60" r:id="rId108"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E61" r:id="rId109"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E62" r:id="rId110"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E63" r:id="rId111"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E55" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E56" r:id="rId103"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E57" r:id="rId104"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E58" r:id="rId105"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E59" r:id="rId106"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E60" r:id="rId107"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E61" r:id="rId108"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E62" r:id="rId109"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E63" r:id="rId110"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F63" r:id="rId111"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E64" r:id="rId112"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F64" r:id="rId113"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E65" r:id="rId114"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E65" r:id="rId113"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F65" r:id="rId114"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E66" r:id="rId115"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F66" r:id="rId116"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E67" r:id="rId117"/>
@@ -3132,22 +3100,20 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E69" r:id="rId121"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F69" r:id="rId122"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E70" r:id="rId123"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F70" r:id="rId124"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E71" r:id="rId125"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E72" r:id="rId124"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F72" r:id="rId125"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E73" r:id="rId126"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F73" r:id="rId127"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E74" r:id="rId128"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E75" r:id="rId129"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E76" r:id="rId130"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E77" r:id="rId131"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E78" r:id="rId132"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E79" r:id="rId133"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E80" r:id="rId134"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E81" r:id="rId135"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E82" r:id="rId136"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E83" r:id="rId137"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E84" r:id="rId138"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E85" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E74" r:id="rId127"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E75" r:id="rId128"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E76" r:id="rId129"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E77" r:id="rId130"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E78" r:id="rId131"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E79" r:id="rId132"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E80" r:id="rId133"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E81" r:id="rId134"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E82" r:id="rId135"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E83" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E84" r:id="rId137"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>